<commit_message>
update. going to migrate to Proj folder
</commit_message>
<xml_diff>
--- a/Ancillary Files/Logger Serial Site List.xlsx
+++ b/Ancillary Files/Logger Serial Site List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\2022_County_LowFlow\Ancillary Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6990DD8-71B5-4500-BC45-6A8E14D9BE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FD6B87-620D-4C18-B02C-41AD719D3B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="420" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{53F71B59-5793-43B2-BCD6-E04FB72ECA05}"/>
+    <workbookView xWindow="-25320" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{53F71B59-5793-43B2-BCD6-E04FB72ECA05}"/>
   </bookViews>
   <sheets>
     <sheet name="by logger" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
   <si>
     <t>06-02265</t>
   </si>
@@ -290,13 +290,22 @@
   </si>
   <si>
     <t>SDR-035</t>
+  </si>
+  <si>
+    <t>06-01636</t>
+  </si>
+  <si>
+    <t>LN-K01-12177-1</t>
+  </si>
+  <si>
+    <t>1685401568; 1286503872</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +350,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -393,6 +408,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09575956-55C0-4B64-9B3F-595498DE8D83}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1113,7 +1131,15 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="A34" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
@@ -1207,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027BE51-06E4-4234-8806-914AFBC23B71}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,6 +1712,20 @@
       </c>
       <c r="D37" s="13" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="11">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
July update and removing SDR-098 from list
SDR-098 will not be monitored due to ongoing repairs
</commit_message>
<xml_diff>
--- a/Ancillary Files/Logger Serial Site List.xlsx
+++ b/Ancillary Files/Logger Serial Site List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\2022_County_LowFlow\Ancillary Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FD6B87-620D-4C18-B02C-41AD719D3B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753353CA-3E20-491E-8185-B1192E489124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{53F71B59-5793-43B2-BCD6-E04FB72ECA05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{53F71B59-5793-43B2-BCD6-E04FB72ECA05}"/>
   </bookViews>
   <sheets>
     <sheet name="by logger" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="85">
   <si>
     <t>06-02265</t>
   </si>
@@ -70,9 +70,6 @@
     <t>06-02190</t>
   </si>
   <si>
-    <t>06-02246</t>
-  </si>
-  <si>
     <t>06-02192</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
   </si>
   <si>
     <t>SDR-034A</t>
-  </si>
-  <si>
-    <t>SDR-098</t>
   </si>
   <si>
     <t>SDR-098B</t>
@@ -825,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09575956-55C0-4B64-9B3F-595498DE8D83}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,13 +835,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -863,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="7">
         <v>1354303492</v>
@@ -890,7 +884,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -922,7 +916,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -930,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -938,7 +932,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,7 +940,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +948,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,10 +959,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,7 +975,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +983,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1352203377</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -997,10 +994,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="7">
-        <v>1352203377</v>
+        <v>1345303411</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,10 +1005,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1345303411</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1019,7 +1013,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,7 +1021,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,7 +1029,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1043,7 +1037,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1348703321</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1051,10 +1048,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="7">
-        <v>1348703321</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1062,7 +1056,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1070,10 +1067,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1081,7 +1075,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1083,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,49 +1091,44 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1706603740</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1706603740</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>69</v>
+    </row>
+    <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>82</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
@@ -1219,12 +1208,9 @@
     <row r="60" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
-    <sortCondition ref="B2:B31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
+    <sortCondition ref="B2:B30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1233,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5027BE51-06E4-4234-8806-914AFBC23B71}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,57 +1235,57 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -1308,184 +1294,186 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="10">
+        <v>3</v>
+      </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10">
-        <v>4</v>
-      </c>
+      <c r="C16" s="9"/>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="10">
+        <v>3</v>
+      </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
@@ -1494,238 +1482,224 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10">
-        <v>3</v>
-      </c>
+      <c r="C21" s="9"/>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="10">
+        <v>3</v>
+      </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="10">
-        <v>3</v>
-      </c>
+      <c r="C26" s="9"/>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="9">
-        <v>1</v>
-      </c>
+      <c r="C28" s="9"/>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>55</v>
+      <c r="A32" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="C32" s="11">
+        <v>4</v>
+      </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C34" s="11">
         <v>3</v>
       </c>
-      <c r="D34" t="s">
-        <v>77</v>
+      <c r="D34" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="13" t="s">
         <v>79</v>
       </c>
       <c r="C35" s="11">
         <v>3</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="C36" s="11">
         <v>3</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
         <v>82</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="C37" s="11">
         <v>3</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="11">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>77</v>
+      <c r="D37" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1738,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F405E8-A134-4AB0-8D02-837C997BDDEB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1750,26 +1724,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>